<commit_message>
A variety of edits. Including one that involved figuring out what UTF-8 mu actually is.
Also stopped printing csv files that are larger than 50,000 lines.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/USDA GFS IMPACT V17.xlsx
+++ b/data-raw/NutrientData/USDA GFS IMPACT V17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="720" windowWidth="26540" windowHeight="12120"/>
+    <workbookView xWindow="-100" yWindow="800" windowWidth="26540" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -650,9 +650,6 @@
     <t>cholesterol_mg</t>
   </si>
   <si>
-    <t>vit_d_µg</t>
-  </si>
-  <si>
     <t>totalfiber_g</t>
   </si>
   <si>
@@ -1149,6 +1146,9 @@
   </si>
   <si>
     <t>folate_µg_cr</t>
+  </si>
+  <si>
+    <t>vit_d_μg</t>
   </si>
 </sst>
 </file>
@@ -4220,10 +4220,10 @@
   <dimension ref="A1:BL65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AL1" sqref="AL1:AL1048576"/>
+      <selection pane="bottomRight" activeCell="AX3" sqref="AT1:BE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4269,9 +4269,21 @@
     <col min="42" max="42" width="11.1640625" style="13" customWidth="1"/>
     <col min="43" max="43" width="11" style="13" customWidth="1"/>
     <col min="44" max="45" width="9.6640625" style="13" customWidth="1"/>
-    <col min="46" max="46" width="9.1640625" style="13" customWidth="1"/>
-    <col min="47" max="47" width="9.1640625" style="32" customWidth="1"/>
-    <col min="48" max="16384" width="8.6640625" style="13"/>
+    <col min="46" max="46" width="17.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.1640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="33.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="58" max="61" width="8.6640625" style="13"/>
+    <col min="62" max="62" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:64" s="50" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4397,7 +4409,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>93</v>
@@ -4519,13 +4531,13 @@
         <v>38</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F3" s="41" t="s">
         <v>146</v>
@@ -4549,58 +4561,58 @@
         <v>173</v>
       </c>
       <c r="M3" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="N3" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="O3" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="O3" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="R3" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="Q3" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="R3" s="37" t="s">
+      <c r="S3" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="U3" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="37" t="s">
+      <c r="V3" s="37" t="s">
         <v>199</v>
-      </c>
-      <c r="V3" s="37" t="s">
-        <v>200</v>
       </c>
       <c r="W3" s="37" t="s">
         <v>174</v>
       </c>
       <c r="X3" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y3" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="Y3" s="37" t="s">
-        <v>329</v>
-      </c>
       <c r="Z3" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>143</v>
       </c>
       <c r="AB3" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC3" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AD3" s="37" t="s">
         <v>203</v>
-      </c>
-      <c r="AD3" s="37" t="s">
-        <v>204</v>
       </c>
       <c r="AE3" s="37" t="s">
         <v>181</v>
@@ -4609,7 +4621,7 @@
         <v>182</v>
       </c>
       <c r="AG3" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AH3" s="37" t="s">
         <v>183</v>
@@ -4621,7 +4633,7 @@
         <v>184</v>
       </c>
       <c r="AK3" s="37" t="s">
-        <v>190</v>
+        <v>352</v>
       </c>
       <c r="AL3" s="37" t="s">
         <v>185</v>
@@ -4645,13 +4657,13 @@
         <v>154</v>
       </c>
       <c r="AS3" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="AT3" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="AT3" s="11" t="s">
-        <v>206</v>
-      </c>
       <c r="AU3" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AV3" s="63" t="s">
         <v>158</v>
@@ -4660,7 +4672,7 @@
         <v>176</v>
       </c>
       <c r="AX3" s="63" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AY3" s="63" t="s">
         <v>177</v>
@@ -4672,31 +4684,31 @@
         <v>179</v>
       </c>
       <c r="BB3" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="BC3" s="63" t="s">
         <v>207</v>
       </c>
-      <c r="BC3" s="63" t="s">
+      <c r="BD3" s="63" t="s">
+        <v>351</v>
+      </c>
+      <c r="BE3" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="BF3" s="63" t="s">
         <v>208</v>
       </c>
-      <c r="BD3" s="63" t="s">
-        <v>352</v>
-      </c>
-      <c r="BE3" s="63" t="s">
-        <v>213</v>
-      </c>
-      <c r="BF3" s="63" t="s">
+      <c r="BG3" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="BH3" s="63" t="s">
         <v>209</v>
       </c>
-      <c r="BG3" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="BH3" s="63" t="s">
+      <c r="BI3" s="63" t="s">
+        <v>350</v>
+      </c>
+      <c r="BJ3" s="63" t="s">
         <v>210</v>
-      </c>
-      <c r="BI3" s="63" t="s">
-        <v>351</v>
-      </c>
-      <c r="BJ3" s="63" t="s">
-        <v>211</v>
       </c>
       <c r="BK3" s="63" t="s">
         <v>172</v>
@@ -4720,10 +4732,10 @@
         <v>39</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14">
@@ -4828,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="AV5" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW5" s="63"/>
       <c r="AX5" s="63"/>
@@ -4855,17 +4867,17 @@
         <v>40</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14">
         <v>12101001</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H6" s="28">
         <v>100</v>
@@ -5026,7 +5038,7 @@
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>41</v>
@@ -5230,17 +5242,17 @@
         <v>42</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14">
         <v>18101045</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H8" s="28">
         <v>100</v>
@@ -5403,10 +5415,10 @@
         <v>43</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14">
@@ -5509,7 +5521,7 @@
         <v>3142</v>
       </c>
       <c r="AV9" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW9" s="63"/>
       <c r="AX9" s="63"/>
@@ -5536,10 +5548,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14">
@@ -5706,10 +5718,10 @@
         <v>78</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -5872,10 +5884,10 @@
         <v>45</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14">
@@ -5978,7 +5990,7 @@
         <v>230</v>
       </c>
       <c r="AV12" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW12" s="63"/>
       <c r="AX12" s="63"/>
@@ -6005,10 +6017,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="66"/>
@@ -6159,10 +6171,10 @@
         <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14">
@@ -6332,10 +6344,10 @@
         <v>47</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14">
@@ -6441,7 +6453,7 @@
         <v>5019</v>
       </c>
       <c r="AV15" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW15" s="63">
         <v>1</v>
@@ -6500,10 +6512,10 @@
         <v>48</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14">
@@ -6609,7 +6621,7 @@
         <v>2202</v>
       </c>
       <c r="AV16" s="63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AW16" s="63">
         <v>0.85</v>
@@ -6669,7 +6681,7 @@
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>49</v>
@@ -6678,7 +6690,7 @@
         <v>18102056</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H17" s="28">
         <f>[2]Sheet1!$B$4</f>
@@ -6817,7 +6829,7 @@
         <v>1004</v>
       </c>
       <c r="AV17" s="63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AW17" s="63">
         <v>0.6</v>
@@ -6876,10 +6888,10 @@
         <v>81</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14">
@@ -7044,10 +7056,10 @@
         <v>50</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="59">
@@ -7215,10 +7227,10 @@
         <v>51</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14">
@@ -7318,7 +7330,7 @@
       <c r="AT20" s="13"/>
       <c r="AU20" s="32"/>
       <c r="AV20" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW20" s="63"/>
       <c r="AX20" s="63"/>
@@ -7345,10 +7357,10 @@
         <v>52</v>
       </c>
       <c r="C21" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>272</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>273</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14">
@@ -7508,7 +7520,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>53</v>
@@ -7713,7 +7725,7 @@
         <v>54</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>54</v>
@@ -7919,10 +7931,10 @@
         <v>83</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
@@ -7931,7 +7943,7 @@
         <v>86</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J24" s="65"/>
       <c r="L24" s="37">
@@ -8094,7 +8106,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>84</v>
@@ -8240,7 +8252,7 @@
         <v>2202</v>
       </c>
       <c r="AV25" s="63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AW25" s="63">
         <v>0.85</v>
@@ -8299,10 +8311,10 @@
         <v>86</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -8453,10 +8465,10 @@
         <v>56</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -8560,7 +8572,7 @@
         <v>5019</v>
       </c>
       <c r="AV27" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW27" s="63">
         <v>1</v>
@@ -8619,10 +8631,10 @@
         <v>76</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="68"/>
@@ -8787,10 +8799,10 @@
         <v>57</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14">
@@ -8894,7 +8906,7 @@
         <v>5019</v>
       </c>
       <c r="AV29" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW29" s="63">
         <v>1</v>
@@ -8953,17 +8965,17 @@
         <v>58</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14">
         <v>18103095</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H30" s="31">
         <v>100</v>
@@ -9114,10 +9126,10 @@
         <v>59</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14">
@@ -9225,7 +9237,7 @@
         <v>3308</v>
       </c>
       <c r="AV31" s="63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AW31" s="63">
         <v>0.8</v>
@@ -9284,10 +9296,10 @@
         <v>60</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14">
@@ -9454,10 +9466,10 @@
         <v>61</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14">
@@ -9622,7 +9634,7 @@
         <v>75</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>75</v>
@@ -9766,7 +9778,7 @@
         <v>5019</v>
       </c>
       <c r="AV34" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW34" s="63">
         <v>1</v>
@@ -9993,10 +10005,10 @@
         <v>62</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14">
@@ -10105,7 +10117,7 @@
         <v>5019</v>
       </c>
       <c r="AV36" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW36" s="63">
         <v>1</v>
@@ -10164,10 +10176,10 @@
         <v>63</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14">
@@ -10273,7 +10285,7 @@
         <v>5019</v>
       </c>
       <c r="AV37" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW37" s="63">
         <v>1</v>
@@ -10332,10 +10344,10 @@
         <v>64</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14">
@@ -10440,7 +10452,7 @@
         <v>0</v>
       </c>
       <c r="AV38" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW38" s="63"/>
       <c r="AX38" s="63"/>
@@ -10467,10 +10479,10 @@
         <v>65</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -10630,10 +10642,10 @@
         <v>74</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14">
@@ -10798,7 +10810,7 @@
         <v>90</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>90</v>
@@ -10940,7 +10952,7 @@
       </c>
       <c r="AT41" s="16"/>
       <c r="AV41" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW41" s="63"/>
       <c r="AX41" s="63"/>
@@ -10967,10 +10979,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14">
@@ -11076,7 +11088,7 @@
         <v>0</v>
       </c>
       <c r="AV42" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW42" s="63"/>
       <c r="AX42" s="63"/>
@@ -11103,17 +11115,17 @@
         <v>66</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="14">
         <v>24302043</v>
       </c>
       <c r="G43" s="57" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H43" s="31">
         <v>72</v>
@@ -11376,7 +11388,7 @@
         <v>0</v>
       </c>
       <c r="AV44" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW44" s="63"/>
       <c r="AX44" s="63"/>
@@ -11404,7 +11416,7 @@
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>72</v>
@@ -11549,7 +11561,7 @@
         <v>0</v>
       </c>
       <c r="AV45" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW45" s="63"/>
       <c r="AX45" s="63"/>
@@ -11576,7 +11588,7 @@
         <v>69</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>69</v>
@@ -11724,7 +11736,7 @@
         <v>5019</v>
       </c>
       <c r="AV46" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW46" s="63">
         <v>1</v>
@@ -11783,10 +11795,10 @@
         <v>68</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14">
@@ -11892,7 +11904,7 @@
         <v>5019</v>
       </c>
       <c r="AV47" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW47" s="63">
         <v>1</v>
@@ -11952,7 +11964,7 @@
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>70</v>
@@ -12100,7 +12112,7 @@
         <v>3771</v>
       </c>
       <c r="AV48" s="63" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AW48" s="63">
         <v>0.9</v>
@@ -12159,10 +12171,10 @@
         <v>71</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14">
@@ -12315,10 +12327,10 @@
         <v>55</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14">
@@ -12479,16 +12491,16 @@
     </row>
     <row r="51" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="53"/>
@@ -12496,7 +12508,7 @@
         <v>87</v>
       </c>
       <c r="I51" s="71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L51" s="2">
         <v>83.01</v>
@@ -12597,7 +12609,7 @@
         <v>2753</v>
       </c>
       <c r="AV51" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AW51" s="63">
         <v>0.9</v>
@@ -12650,17 +12662,17 @@
     </row>
     <row r="52" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E52" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H52" s="29">
         <f>'[11]Weighted Composition'!$C$201</f>
@@ -12801,7 +12813,7 @@
         <v>2702</v>
       </c>
       <c r="AV52" s="63" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AW52" s="63">
         <v>0.95</v>
@@ -12854,17 +12866,17 @@
     </row>
     <row r="53" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E53" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H53" s="29">
         <f>'[12]Weighted Composition'!$C$121</f>
@@ -13005,7 +13017,7 @@
         <v>2770</v>
       </c>
       <c r="AV53" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW53" s="63">
         <v>0.95</v>
@@ -13058,16 +13070,16 @@
     </row>
     <row r="54" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" s="54" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E54" s="14"/>
       <c r="H54" s="29">
@@ -13157,7 +13169,7 @@
         <v>2455</v>
       </c>
       <c r="AV54" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AW54" s="63">
         <v>0.95</v>
@@ -13210,17 +13222,17 @@
     </row>
     <row r="55" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H55" s="29">
         <f>'[13]Weighted Composition'!$C$382</f>
@@ -13361,7 +13373,7 @@
         <v>2305</v>
       </c>
       <c r="AV55" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AW55" s="63">
         <v>0.9</v>
@@ -13414,16 +13426,16 @@
     </row>
     <row r="56" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
@@ -13515,7 +13527,7 @@
         <v>2305</v>
       </c>
       <c r="AV56" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AW56" s="63">
         <v>0.9</v>
@@ -13568,17 +13580,17 @@
     </row>
     <row r="57" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E57" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H57" s="29">
         <f>'[14]Weighted Composition'!$C$236</f>
@@ -13719,7 +13731,7 @@
         <v>2305</v>
       </c>
       <c r="AV57" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AW57" s="63">
         <v>0.9</v>
@@ -13772,17 +13784,17 @@
     </row>
     <row r="58" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E58" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H58" s="29">
         <f>'[15]Weighted Composite'!$C$944</f>
@@ -13923,7 +13935,7 @@
         <v>2305</v>
       </c>
       <c r="AV58" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AW58" s="63">
         <v>0.9</v>
@@ -13976,17 +13988,17 @@
     </row>
     <row r="59" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E59" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H59" s="29">
         <f>AVERAGE(H57:H58)</f>
@@ -14127,7 +14139,7 @@
         <v>2305</v>
       </c>
       <c r="AV59" s="63" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AW59" s="63">
         <v>0.9</v>
@@ -14180,16 +14192,16 @@
     </row>
     <row r="60" spans="1:64" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="53"/>
@@ -14280,7 +14292,7 @@
         <v>710</v>
       </c>
       <c r="AV60" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW60" s="63"/>
       <c r="AX60" s="63"/>
@@ -14301,16 +14313,16 @@
     </row>
     <row r="61" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A61" s="75" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B61" s="76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E61" s="14"/>
       <c r="H61" s="31">
@@ -14413,7 +14425,7 @@
       </c>
       <c r="AU61" s="74"/>
       <c r="AV61" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW61" s="63"/>
       <c r="AX61" s="63"/>
@@ -14434,16 +14446,16 @@
     </row>
     <row r="62" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A62" s="75" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B62" s="76" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E62" s="14"/>
       <c r="H62" s="31">
@@ -14546,7 +14558,7 @@
       </c>
       <c r="AU62" s="74"/>
       <c r="AV62" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW62" s="63"/>
       <c r="AX62" s="63"/>
@@ -14567,16 +14579,16 @@
     </row>
     <row r="63" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A63" s="75" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B63" s="76" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E63" s="14"/>
       <c r="H63" s="31">
@@ -14664,7 +14676,7 @@
       </c>
       <c r="AU63" s="74"/>
       <c r="AV63" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW63" s="63"/>
       <c r="AX63" s="63"/>
@@ -14685,10 +14697,10 @@
     </row>
     <row r="64" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A64" s="75" t="s">
+        <v>345</v>
+      </c>
+      <c r="B64" s="76" t="s">
         <v>346</v>
-      </c>
-      <c r="B64" s="76" t="s">
-        <v>347</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>42</v>
@@ -14846,10 +14858,10 @@
     </row>
     <row r="65" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A65" s="75" t="s">
+        <v>347</v>
+      </c>
+      <c r="B65" s="76" t="s">
         <v>348</v>
-      </c>
-      <c r="B65" s="76" t="s">
-        <v>349</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>70</v>
@@ -14963,7 +14975,7 @@
         <v>3771</v>
       </c>
       <c r="AV65" s="56" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AW65" s="56">
         <v>0.9</v>

</xml_diff>

<commit_message>
significant cleanup to nutCalcsGraphing.R but probably still not working yet.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/USDA GFS IMPACT V17.xlsx
+++ b/data-raw/NutrientData/USDA GFS IMPACT V17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="800" windowWidth="26540" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="26540" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -596,9 +596,6 @@
     <t>IMPACT to nutrients unit conversion rate (%)</t>
   </si>
   <si>
-    <t>vit_e_cr</t>
-  </si>
-  <si>
     <t>water_g</t>
   </si>
   <si>
@@ -1149,6 +1146,9 @@
   </si>
   <si>
     <t>vit_d_μg</t>
+  </si>
+  <si>
+    <t>vit_e_mg_cr</t>
   </si>
 </sst>
 </file>
@@ -4220,10 +4220,10 @@
   <dimension ref="A1:BL65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="AV4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="BD4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AX3" sqref="AT1:BE1048576"/>
+      <selection pane="bottomRight" activeCell="BK3" sqref="BK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>93</v>
@@ -4531,13 +4531,13 @@
         <v>38</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F3" s="41" t="s">
         <v>146</v>
@@ -4558,163 +4558,163 @@
         <v>151</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="N3" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q3" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="R3" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="V3" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="W3" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="M3" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="N3" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="O3" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q3" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="R3" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="T3" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="U3" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="V3" s="37" t="s">
+      <c r="X3" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y3" s="37" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z3" s="37" t="s">
         <v>199</v>
-      </c>
-      <c r="W3" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="X3" s="37" t="s">
-        <v>327</v>
-      </c>
-      <c r="Y3" s="37" t="s">
-        <v>328</v>
-      </c>
-      <c r="Z3" s="37" t="s">
-        <v>200</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>143</v>
       </c>
       <c r="AB3" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC3" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="AC3" s="37" t="s">
+      <c r="AD3" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="AD3" s="37" t="s">
-        <v>203</v>
-      </c>
       <c r="AE3" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF3" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="AF3" s="37" t="s">
+      <c r="AG3" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="AH3" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="AG3" s="37" t="s">
-        <v>213</v>
-      </c>
-      <c r="AH3" s="37" t="s">
+      <c r="AI3" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ3" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="AI3" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="AJ3" s="37" t="s">
+      <c r="AK3" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="AL3" s="37" t="s">
         <v>184</v>
-      </c>
-      <c r="AK3" s="37" t="s">
-        <v>352</v>
-      </c>
-      <c r="AL3" s="37" t="s">
-        <v>185</v>
       </c>
       <c r="AM3" s="13" t="s">
         <v>144</v>
       </c>
       <c r="AN3" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO3" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="AO3" s="37" t="s">
+      <c r="AP3" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="AP3" s="37" t="s">
+      <c r="AQ3" s="37" t="s">
         <v>188</v>
-      </c>
-      <c r="AQ3" s="37" t="s">
-        <v>189</v>
       </c>
       <c r="AR3" s="13" t="s">
         <v>154</v>
       </c>
       <c r="AS3" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="AT3" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="AT3" s="11" t="s">
-        <v>205</v>
-      </c>
       <c r="AU3" s="34" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AV3" s="63" t="s">
         <v>158</v>
       </c>
       <c r="AW3" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX3" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="AY3" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="AX3" s="63" t="s">
+      <c r="AZ3" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA3" s="63" t="s">
+        <v>178</v>
+      </c>
+      <c r="BB3" s="63" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC3" s="63" t="s">
+        <v>206</v>
+      </c>
+      <c r="BD3" s="63" t="s">
+        <v>350</v>
+      </c>
+      <c r="BE3" s="63" t="s">
+        <v>211</v>
+      </c>
+      <c r="BF3" s="63" t="s">
+        <v>207</v>
+      </c>
+      <c r="BG3" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="BH3" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="BI3" s="63" t="s">
         <v>349</v>
       </c>
-      <c r="AY3" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ3" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="BA3" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB3" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="BC3" s="63" t="s">
-        <v>207</v>
-      </c>
-      <c r="BD3" s="63" t="s">
-        <v>351</v>
-      </c>
-      <c r="BE3" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="BF3" s="63" t="s">
-        <v>208</v>
-      </c>
-      <c r="BG3" s="63" t="s">
-        <v>211</v>
-      </c>
-      <c r="BH3" s="63" t="s">
+      <c r="BJ3" s="63" t="s">
         <v>209</v>
       </c>
-      <c r="BI3" s="63" t="s">
-        <v>350</v>
-      </c>
-      <c r="BJ3" s="63" t="s">
-        <v>210</v>
-      </c>
       <c r="BK3" s="63" t="s">
-        <v>172</v>
+        <v>352</v>
       </c>
       <c r="BL3" s="63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4732,10 +4732,10 @@
         <v>39</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14">
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="AV5" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW5" s="63"/>
       <c r="AX5" s="63"/>
@@ -4867,17 +4867,17 @@
         <v>40</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14">
         <v>12101001</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H6" s="28">
         <v>100</v>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>41</v>
@@ -5242,17 +5242,17 @@
         <v>42</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14">
         <v>18101045</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H8" s="28">
         <v>100</v>
@@ -5415,10 +5415,10 @@
         <v>43</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14">
@@ -5521,7 +5521,7 @@
         <v>3142</v>
       </c>
       <c r="AV9" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW9" s="63"/>
       <c r="AX9" s="63"/>
@@ -5548,10 +5548,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14">
@@ -5718,10 +5718,10 @@
         <v>78</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -5884,10 +5884,10 @@
         <v>45</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14">
@@ -5990,7 +5990,7 @@
         <v>230</v>
       </c>
       <c r="AV12" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW12" s="63"/>
       <c r="AX12" s="63"/>
@@ -6017,10 +6017,10 @@
         <v>80</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="66"/>
@@ -6171,10 +6171,10 @@
         <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14">
@@ -6344,10 +6344,10 @@
         <v>47</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14">
@@ -6453,7 +6453,7 @@
         <v>5019</v>
       </c>
       <c r="AV15" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW15" s="63">
         <v>1</v>
@@ -6512,10 +6512,10 @@
         <v>48</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14">
@@ -6621,7 +6621,7 @@
         <v>2202</v>
       </c>
       <c r="AV16" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW16" s="63">
         <v>0.85</v>
@@ -6681,7 +6681,7 @@
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>49</v>
@@ -6690,7 +6690,7 @@
         <v>18102056</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H17" s="28">
         <f>[2]Sheet1!$B$4</f>
@@ -6829,7 +6829,7 @@
         <v>1004</v>
       </c>
       <c r="AV17" s="63" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AW17" s="63">
         <v>0.6</v>
@@ -6888,10 +6888,10 @@
         <v>81</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14">
@@ -7056,10 +7056,10 @@
         <v>50</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="59">
@@ -7227,10 +7227,10 @@
         <v>51</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14">
@@ -7330,7 +7330,7 @@
       <c r="AT20" s="13"/>
       <c r="AU20" s="32"/>
       <c r="AV20" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW20" s="63"/>
       <c r="AX20" s="63"/>
@@ -7357,10 +7357,10 @@
         <v>52</v>
       </c>
       <c r="C21" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>272</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14">
@@ -7520,7 +7520,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>53</v>
@@ -7725,7 +7725,7 @@
         <v>54</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>54</v>
@@ -7931,10 +7931,10 @@
         <v>83</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
@@ -7943,7 +7943,7 @@
         <v>86</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J24" s="65"/>
       <c r="L24" s="37">
@@ -8106,7 +8106,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>84</v>
@@ -8252,7 +8252,7 @@
         <v>2202</v>
       </c>
       <c r="AV25" s="63" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AW25" s="63">
         <v>0.85</v>
@@ -8311,10 +8311,10 @@
         <v>86</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -8465,10 +8465,10 @@
         <v>56</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -8572,7 +8572,7 @@
         <v>5019</v>
       </c>
       <c r="AV27" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW27" s="63">
         <v>1</v>
@@ -8631,10 +8631,10 @@
         <v>76</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="68"/>
@@ -8799,10 +8799,10 @@
         <v>57</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14">
@@ -8906,7 +8906,7 @@
         <v>5019</v>
       </c>
       <c r="AV29" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW29" s="63">
         <v>1</v>
@@ -8965,17 +8965,17 @@
         <v>58</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14">
         <v>18103095</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H30" s="31">
         <v>100</v>
@@ -9126,10 +9126,10 @@
         <v>59</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14">
@@ -9237,7 +9237,7 @@
         <v>3308</v>
       </c>
       <c r="AV31" s="63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AW31" s="63">
         <v>0.8</v>
@@ -9296,10 +9296,10 @@
         <v>60</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14">
@@ -9466,10 +9466,10 @@
         <v>61</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14">
@@ -9634,7 +9634,7 @@
         <v>75</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>75</v>
@@ -9778,7 +9778,7 @@
         <v>5019</v>
       </c>
       <c r="AV34" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW34" s="63">
         <v>1</v>
@@ -10005,10 +10005,10 @@
         <v>62</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14">
@@ -10117,7 +10117,7 @@
         <v>5019</v>
       </c>
       <c r="AV36" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW36" s="63">
         <v>1</v>
@@ -10176,10 +10176,10 @@
         <v>63</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14">
@@ -10285,7 +10285,7 @@
         <v>5019</v>
       </c>
       <c r="AV37" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW37" s="63">
         <v>1</v>
@@ -10344,10 +10344,10 @@
         <v>64</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14">
@@ -10452,7 +10452,7 @@
         <v>0</v>
       </c>
       <c r="AV38" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW38" s="63"/>
       <c r="AX38" s="63"/>
@@ -10479,10 +10479,10 @@
         <v>65</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -10642,10 +10642,10 @@
         <v>74</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14">
@@ -10810,7 +10810,7 @@
         <v>90</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>90</v>
@@ -10952,7 +10952,7 @@
       </c>
       <c r="AT41" s="16"/>
       <c r="AV41" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW41" s="63"/>
       <c r="AX41" s="63"/>
@@ -10979,10 +10979,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14">
@@ -11088,7 +11088,7 @@
         <v>0</v>
       </c>
       <c r="AV42" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW42" s="63"/>
       <c r="AX42" s="63"/>
@@ -11115,17 +11115,17 @@
         <v>66</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="14">
         <v>24302043</v>
       </c>
       <c r="G43" s="57" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H43" s="31">
         <v>72</v>
@@ -11388,7 +11388,7 @@
         <v>0</v>
       </c>
       <c r="AV44" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW44" s="63"/>
       <c r="AX44" s="63"/>
@@ -11416,7 +11416,7 @@
       </c>
       <c r="C45" s="27"/>
       <c r="D45" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>72</v>
@@ -11561,7 +11561,7 @@
         <v>0</v>
       </c>
       <c r="AV45" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW45" s="63"/>
       <c r="AX45" s="63"/>
@@ -11588,7 +11588,7 @@
         <v>69</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>69</v>
@@ -11736,7 +11736,7 @@
         <v>5019</v>
       </c>
       <c r="AV46" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW46" s="63">
         <v>1</v>
@@ -11795,10 +11795,10 @@
         <v>68</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14">
@@ -11904,7 +11904,7 @@
         <v>5019</v>
       </c>
       <c r="AV47" s="63" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AW47" s="63">
         <v>1</v>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>70</v>
@@ -12112,7 +12112,7 @@
         <v>3771</v>
       </c>
       <c r="AV48" s="63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AW48" s="63">
         <v>0.9</v>
@@ -12171,10 +12171,10 @@
         <v>71</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="14">
@@ -12327,10 +12327,10 @@
         <v>55</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14">
@@ -12491,16 +12491,16 @@
     </row>
     <row r="51" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="53"/>
@@ -12508,7 +12508,7 @@
         <v>87</v>
       </c>
       <c r="I51" s="71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L51" s="2">
         <v>83.01</v>
@@ -12609,7 +12609,7 @@
         <v>2753</v>
       </c>
       <c r="AV51" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AW51" s="63">
         <v>0.9</v>
@@ -12662,17 +12662,17 @@
     </row>
     <row r="52" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E52" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H52" s="29">
         <f>'[11]Weighted Composition'!$C$201</f>
@@ -12813,7 +12813,7 @@
         <v>2702</v>
       </c>
       <c r="AV52" s="63" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AW52" s="63">
         <v>0.95</v>
@@ -12866,17 +12866,17 @@
     </row>
     <row r="53" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E53" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H53" s="29">
         <f>'[12]Weighted Composition'!$C$121</f>
@@ -13017,7 +13017,7 @@
         <v>2770</v>
       </c>
       <c r="AV53" s="63" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AW53" s="63">
         <v>0.95</v>
@@ -13070,16 +13070,16 @@
     </row>
     <row r="54" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C54" s="54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E54" s="14"/>
       <c r="H54" s="29">
@@ -13169,7 +13169,7 @@
         <v>2455</v>
       </c>
       <c r="AV54" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AW54" s="63">
         <v>0.95</v>
@@ -13222,17 +13222,17 @@
     </row>
     <row r="55" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H55" s="29">
         <f>'[13]Weighted Composition'!$C$382</f>
@@ -13373,7 +13373,7 @@
         <v>2305</v>
       </c>
       <c r="AV55" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW55" s="63">
         <v>0.9</v>
@@ -13426,16 +13426,16 @@
     </row>
     <row r="56" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
@@ -13527,7 +13527,7 @@
         <v>2305</v>
       </c>
       <c r="AV56" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW56" s="63">
         <v>0.9</v>
@@ -13580,17 +13580,17 @@
     </row>
     <row r="57" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E57" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H57" s="29">
         <f>'[14]Weighted Composition'!$C$236</f>
@@ -13731,7 +13731,7 @@
         <v>2305</v>
       </c>
       <c r="AV57" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW57" s="63">
         <v>0.9</v>
@@ -13784,17 +13784,17 @@
     </row>
     <row r="58" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E58" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H58" s="29">
         <f>'[15]Weighted Composite'!$C$944</f>
@@ -13935,7 +13935,7 @@
         <v>2305</v>
       </c>
       <c r="AV58" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW58" s="63">
         <v>0.9</v>
@@ -13988,17 +13988,17 @@
     </row>
     <row r="59" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E59" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H59" s="29">
         <f>AVERAGE(H57:H58)</f>
@@ -14139,7 +14139,7 @@
         <v>2305</v>
       </c>
       <c r="AV59" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AW59" s="63">
         <v>0.9</v>
@@ -14192,16 +14192,16 @@
     </row>
     <row r="60" spans="1:64" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="53"/>
@@ -14292,7 +14292,7 @@
         <v>710</v>
       </c>
       <c r="AV60" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW60" s="63"/>
       <c r="AX60" s="63"/>
@@ -14313,16 +14313,16 @@
     </row>
     <row r="61" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A61" s="75" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B61" s="76" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E61" s="14"/>
       <c r="H61" s="31">
@@ -14425,7 +14425,7 @@
       </c>
       <c r="AU61" s="74"/>
       <c r="AV61" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW61" s="63"/>
       <c r="AX61" s="63"/>
@@ -14446,16 +14446,16 @@
     </row>
     <row r="62" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A62" s="75" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B62" s="76" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E62" s="14"/>
       <c r="H62" s="31">
@@ -14558,7 +14558,7 @@
       </c>
       <c r="AU62" s="74"/>
       <c r="AV62" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW62" s="63"/>
       <c r="AX62" s="63"/>
@@ -14579,16 +14579,16 @@
     </row>
     <row r="63" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A63" s="75" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B63" s="76" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E63" s="14"/>
       <c r="H63" s="31">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="AU63" s="74"/>
       <c r="AV63" s="63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW63" s="63"/>
       <c r="AX63" s="63"/>
@@ -14697,10 +14697,10 @@
     </row>
     <row r="64" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A64" s="75" t="s">
+        <v>344</v>
+      </c>
+      <c r="B64" s="76" t="s">
         <v>345</v>
-      </c>
-      <c r="B64" s="76" t="s">
-        <v>346</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>42</v>
@@ -14858,10 +14858,10 @@
     </row>
     <row r="65" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A65" s="75" t="s">
+        <v>346</v>
+      </c>
+      <c r="B65" s="76" t="s">
         <v>347</v>
-      </c>
-      <c r="B65" s="76" t="s">
-        <v>348</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>70</v>
@@ -14975,7 +14975,7 @@
         <v>3771</v>
       </c>
       <c r="AV65" s="56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AW65" s="56">
         <v>0.9</v>

</xml_diff>